<commit_message>
Signed-off-by: Flavio Tobler <flavio.to@hispeed.ch>
</commit_message>
<xml_diff>
--- a/Administratives/Zeitplanung.xlsx
+++ b/Administratives/Zeitplanung.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2" xr2:uid="{A66CC244-F7B9-4555-97EB-3609311084C7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{A66CC244-F7B9-4555-97EB-3609311084C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan_FT_Soll" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -510,12 +510,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,16 +526,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -559,24 +547,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -650,6 +620,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -969,7 +957,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:J9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,78 +968,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="6">
+        <f>C5+C6+C7+C8+C9</f>
         <v>3</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:J3" si="0">D5+D6+D7+D8+D9</f>
         <v>5</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="6">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1059,83 +1055,87 @@
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
+        <f>B6+B5+B7+B8+B9</f>
         <v>60</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="53"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="18">
+        <f>C5+D5+E5+F5+G5+H5+I5+J5</f>
         <v>30</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="32">
         <v>3</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="33">
         <v>5</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="33">
         <v>8</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="33">
         <v>8</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="33">
         <v>6</v>
       </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="55"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="18">
+        <f t="shared" ref="B6:B9" si="1">C6+D6+E6+F6+G6+H6+I6+J6</f>
         <v>5</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="43">
+      <c r="C6" s="46"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="33">
         <v>2</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="33">
         <v>3</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="18">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="43">
+      <c r="C7" s="46"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="33">
         <v>5</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="33">
         <v>6</v>
       </c>
-      <c r="J7" s="58">
+      <c r="J7" s="48">
         <v>7</v>
       </c>
     </row>
@@ -1143,19 +1143,20 @@
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="18">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="43">
+      <c r="C8" s="46"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="33">
         <v>1</v>
       </c>
-      <c r="J8" s="58">
+      <c r="J8" s="48">
         <v>1</v>
       </c>
     </row>
@@ -1163,19 +1164,20 @@
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="18">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61">
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="51">
         <v>3</v>
       </c>
-      <c r="J9" s="62">
+      <c r="J9" s="52">
         <v>2</v>
       </c>
     </row>
@@ -1193,7 +1195,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,171 +1206,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="58"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="6">
+        <f>C5+C6+C7+C8+C9</f>
         <v>3</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:J3" si="0">D5+D6+D7+D8+D9</f>
         <v>6</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
+      <c r="F3" s="6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="20">
-        <v>3</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="41"/>
+      <c r="B4" s="17">
+        <f>B5+B6+B7+B8+B9</f>
+        <v>32</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="21">
-        <v>15</v>
-      </c>
-      <c r="C5" s="42">
+      <c r="B5" s="18">
+        <f>C5+D5+E5+F5+G5+H5+I5+J5</f>
+        <v>31</v>
+      </c>
+      <c r="C5" s="32">
         <v>3</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="33">
         <v>6</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="33">
         <v>6</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="45"/>
+      <c r="F5" s="33">
+        <v>8</v>
+      </c>
+      <c r="G5" s="33">
+        <v>8</v>
+      </c>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="45"/>
+      <c r="B6" s="18">
+        <f t="shared" ref="B6:B9" si="1">C6+D6+E6+F6+G6+H6+I6+J6</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="33">
+        <v>1</v>
+      </c>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="45"/>
+      <c r="B7" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="45"/>
+      <c r="B8" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="35"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="50"/>
+      <c r="B9" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="30">
-        <v>3</v>
+      <c r="B10" s="26">
+        <f>B4</f>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1384,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{469A3CF1-99E7-40C8-B132-6A0C415BDF8F}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,78 +1437,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="6">
+        <f>C5+C6+C7+C8+C9</f>
         <v>3</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:J3" si="0">D5+D6+D7+D8+D9</f>
         <v>4</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="6">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1475,83 +1524,87 @@
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
+        <f>B5+B6+B7+B8+B9</f>
         <v>60</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="18">
+        <f>C5+D5+E5+F5+G5+H5+I5+J5</f>
         <v>30</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="32">
         <v>3</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="33">
         <v>4</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="33">
         <v>8</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F5" s="33">
         <v>8</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="33">
         <v>7</v>
       </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="55"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="45"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="18">
+        <f t="shared" ref="B6:B9" si="1">C6+D6+E6+F6+G6+H6+I6+J6</f>
         <v>5</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="43">
+      <c r="C6" s="46"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="33">
         <v>1</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="33">
         <v>4</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="18">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="43">
+      <c r="C7" s="46"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="33">
         <v>4</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="33">
         <v>7</v>
       </c>
-      <c r="J7" s="58">
+      <c r="J7" s="48">
         <v>7</v>
       </c>
     </row>
@@ -1559,19 +1612,20 @@
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="18">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="C8" s="56"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="43">
+      <c r="C8" s="46"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="33">
         <v>1</v>
       </c>
-      <c r="J8" s="58">
+      <c r="J8" s="48">
         <v>1</v>
       </c>
     </row>
@@ -1579,19 +1633,20 @@
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="18">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="61">
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="51">
         <v>3</v>
       </c>
-      <c r="J9" s="62">
+      <c r="J9" s="52">
         <v>2</v>
       </c>
     </row>
@@ -1607,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3033547-3454-487C-8668-F6838D35A31C}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,160 +1674,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="6">
+        <f>C5+C6+C7+C8+C9</f>
         <v>2</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:J3" si="0">D5+D6+D7+D8+D9</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
+        <f>B5+B6+B7+B8+B9</f>
         <v>2</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="18">
+        <f>C5+D5+E5+F5+G5+H5+I5+J5</f>
         <v>2</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="26"/>
+      <c r="C5" s="16">
+        <v>2</v>
+      </c>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="18">
+        <f t="shared" ref="B6:B9" si="1">C6+D6+E6+F6+G6+H6+I6+J6</f>
+        <v>0</v>
+      </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="26"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="26"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="26">
+        <f>B4</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>